<commit_message>
Random work on FileScreen/Menu/XML/PlayerDisplay/Recycle. Perkinites now CS3. All GUIs but FileScreen work. :) :(
</commit_message>
<xml_diff>
--- a/xml/Actors.xlsx
+++ b/xml/Actors.xlsx
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +90,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -180,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -194,57 +200,17 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -456,11 +422,57 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thick">
           <color theme="0"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -496,25 +508,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F8" tableType="xml" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F8" tableType="xml" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A2:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="7">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="5">
       <xmlColumnPr mapId="7" xpath="/Actors/Actor/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Health" name="Health" dataDxfId="6">
+    <tableColumn id="2" uniqueName="Health" name="Health" dataDxfId="4">
       <xmlColumnPr mapId="7" xpath="/Actors/Actor/Health" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Attack" name="Attack" dataDxfId="5">
+    <tableColumn id="3" uniqueName="Attack" name="Attack" dataDxfId="3">
       <xmlColumnPr mapId="7" xpath="/Actors/Actor/Attack" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Defense" name="Defense" dataDxfId="4">
+    <tableColumn id="4" uniqueName="Defense" name="Defense" dataDxfId="2">
       <xmlColumnPr mapId="7" xpath="/Actors/Actor/Defense" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="3">
+    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="1">
       <xmlColumnPr mapId="7" xpath="/Actors/Actor/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Weapon" name="Weapon" dataDxfId="2">
+    <tableColumn id="6" uniqueName="Weapon" name="Weapon" dataDxfId="0">
       <xmlColumnPr mapId="7" xpath="/Actors/Actor/Weapon" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -810,11 +822,12 @@
   <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
@@ -841,82 +854,82 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>75</v>
       </c>
       <c r="C3" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C4" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="A5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="16">
         <v>75</v>
       </c>
-      <c r="C5" s="4">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="16">
+        <v>4</v>
+      </c>
+      <c r="D5" s="16">
         <v>0</v>
       </c>
-      <c r="E5" s="4">
-        <v>20</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>13</v>
+      <c r="E5" s="16">
+        <v>17</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6">
-        <v>100</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="A6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15">
+        <v>60</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15">
         <v>0</v>
       </c>
-      <c r="E6" s="6">
-        <v>16</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>14</v>
+      <c r="E6" s="15">
+        <v>17</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">

</xml_diff>

<commit_message>
That random 'click on MapObject' bug should be gone now hopefully.
</commit_message>
<xml_diff>
--- a/xml/Actors.xlsx
+++ b/xml/Actors.xlsx
@@ -105,18 +105,6 @@
     <t>5+1.5</t>
   </si>
   <si>
-    <t>15+0.2</t>
-  </si>
-  <si>
-    <t>11+0.2</t>
-  </si>
-  <si>
-    <t>12+0.2</t>
-  </si>
-  <si>
-    <t>18+0.2</t>
-  </si>
-  <si>
     <t>Huong V.</t>
   </si>
   <si>
@@ -138,17 +126,29 @@
     <t>Megaphone</t>
   </si>
   <si>
-    <t>14+0.2</t>
-  </si>
-  <si>
-    <t>13+0.2</t>
+    <t>360+5</t>
+  </si>
+  <si>
+    <t>264+5</t>
+  </si>
+  <si>
+    <t>288+5</t>
+  </si>
+  <si>
+    <t>312+5</t>
+  </si>
+  <si>
+    <t>432+5</t>
+  </si>
+  <si>
+    <t>336+5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +162,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -289,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -311,10 +317,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -327,39 +329,43 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -412,6 +418,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -482,6 +489,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -518,6 +526,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -575,58 +584,11 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thick">
           <color theme="0"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -700,33 +662,75 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema5">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Actors">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Actor" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Column1" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Column2" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema6">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Actors">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Actor" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Health" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Attack" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Defense" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Speed" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Weapon" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
   <Map ID="9" Name="Actors_Map" RootElement="Actors" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="10" Name="Actors_Map1" RootElement="Actors" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
   <Map ID="11" Name="Actors_Map2" RootElement="Actors" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="12" Name="Actors_Map3" RootElement="Actors" SchemaID="Schema5" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="13" Name="Actors_Map4" RootElement="Actors" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F10" tableType="xml" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F10" tableType="xml" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7">
   <autoFilter ref="A2:F10"/>
   <tableColumns count="6">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="5">
-      <xmlColumnPr mapId="11" xpath="/Actors/Actor/Name" xmlDataType="string"/>
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="6">
+      <xmlColumnPr mapId="13" xpath="/Actors/Actor/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Health" name="Health" dataDxfId="4">
-      <xmlColumnPr mapId="11" xpath="/Actors/Actor/Health" xmlDataType="string"/>
+    <tableColumn id="2" uniqueName="Health" name="Health" dataDxfId="5">
+      <xmlColumnPr mapId="13" xpath="/Actors/Actor/Health" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Attack" name="Attack" dataDxfId="3">
-      <xmlColumnPr mapId="11" xpath="/Actors/Actor/Attack" xmlDataType="string"/>
+    <tableColumn id="3" uniqueName="Attack" name="Attack" dataDxfId="4">
+      <xmlColumnPr mapId="13" xpath="/Actors/Actor/Attack" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Defense" name="Defense" dataDxfId="2">
-      <xmlColumnPr mapId="11" xpath="/Actors/Actor/Defense" xmlDataType="integer"/>
+    <tableColumn id="4" uniqueName="Defense" name="Defense" dataDxfId="3">
+      <xmlColumnPr mapId="13" xpath="/Actors/Actor/Defense" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="1">
-      <xmlColumnPr mapId="11" xpath="/Actors/Actor/Speed" xmlDataType="string"/>
+    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="2">
+      <xmlColumnPr mapId="13" xpath="/Actors/Actor/Speed" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Weapon" name="Weapon" dataDxfId="0">
-      <xmlColumnPr mapId="11" xpath="/Actors/Actor/Weapon" xmlDataType="string"/>
+    <tableColumn id="6" uniqueName="Weapon" name="Weapon" dataDxfId="1">
+      <xmlColumnPr mapId="13" xpath="/Actors/Actor/Weapon" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1021,13 +1025,14 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1055,19 +1060,19 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1075,19 +1080,19 @@
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1095,19 +1100,19 @@
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="11">
         <v>0</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1115,19 +1120,19 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="8">
         <v>0</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1135,80 +1140,80 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="7">
         <v>0</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>0</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="16" t="s">
+      <c r="E8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>37</v>
       </c>
       <c r="D9" s="7">
         <v>0</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="30" t="s">
+      <c r="E9" s="17" t="s">
         <v>39</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="27" t="s">
+      <c r="A10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="9">
         <v>0</v>
       </c>
-      <c r="E10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>38</v>
+      <c r="E10" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Planning for another big cleanup/restructuring... Q.Q
</commit_message>
<xml_diff>
--- a/xml/Actors.xlsx
+++ b/xml/Actors.xlsx
@@ -114,15 +114,9 @@
     <t>70+5.5</t>
   </si>
   <si>
-    <t>Sophie Q.</t>
-  </si>
-  <si>
     <t>3+1.5</t>
   </si>
   <si>
-    <t>Voice</t>
-  </si>
-  <si>
     <t>Megaphone</t>
   </si>
   <si>
@@ -142,6 +136,12 @@
   </si>
   <si>
     <t>336+5</t>
+  </si>
+  <si>
+    <t>Huilian Q.</t>
+  </si>
+  <si>
+    <t>Microphone</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -337,35 +336,12 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -590,6 +566,30 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -711,25 +711,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F10" tableType="xml" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:F10" tableType="xml" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6">
   <autoFilter ref="A2:F10"/>
   <tableColumns count="6">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="6">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="5">
       <xmlColumnPr mapId="13" xpath="/Actors/Actor/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Health" name="Health" dataDxfId="5">
+    <tableColumn id="2" uniqueName="Health" name="Health" dataDxfId="4">
       <xmlColumnPr mapId="13" xpath="/Actors/Actor/Health" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Attack" name="Attack" dataDxfId="4">
+    <tableColumn id="3" uniqueName="Attack" name="Attack" dataDxfId="3">
       <xmlColumnPr mapId="13" xpath="/Actors/Actor/Attack" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Defense" name="Defense" dataDxfId="3">
+    <tableColumn id="4" uniqueName="Defense" name="Defense" dataDxfId="2">
       <xmlColumnPr mapId="13" xpath="/Actors/Actor/Defense" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="2">
+    <tableColumn id="5" uniqueName="Speed" name="Speed" dataDxfId="1">
       <xmlColumnPr mapId="13" xpath="/Actors/Actor/Speed" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Weapon" name="Weapon" dataDxfId="1">
+    <tableColumn id="6" uniqueName="Weapon" name="Weapon" dataDxfId="0">
       <xmlColumnPr mapId="13" xpath="/Actors/Actor/Weapon" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1025,7 +1025,7 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1049,10 +1049,10 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1060,19 +1060,19 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>0</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1080,39 +1080,39 @@
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="19" t="s">
+      <c r="E5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1120,19 +1120,19 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>0</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="19" t="s">
+      <c r="E6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1140,19 +1140,19 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>0</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="19" t="s">
+      <c r="E7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1160,19 +1160,19 @@
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="19" t="s">
+      <c r="E8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1180,40 +1180,40 @@
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>41</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>